<commit_message>
Aisa bhi hota hai
</commit_message>
<xml_diff>
--- a/Self-practice/TRACKER AND TASKS.xlsx
+++ b/Self-practice/TRACKER AND TASKS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vineet\Desktop\Pyhtonshit\Self-practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3999A46F-E8EA-4073-B7F4-D0A8EB9958EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7E6020-B6B8-4951-A897-AB8C1AF6A719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>To Do</t>
   </si>
@@ -139,6 +139,36 @@
   </si>
   <si>
     <t>SVM and KNN Project (10th and 11tht class material)</t>
+  </si>
+  <si>
+    <t>Flask - house price project</t>
+  </si>
+  <si>
+    <t>Python SQL connection project</t>
+  </si>
+  <si>
+    <t>Feature Engineering and Feature Scaling project</t>
+  </si>
+  <si>
+    <t>KNN is huge (10th SVM and 10th KNN)</t>
+  </si>
+  <si>
+    <t>Naïve Bayes Algo</t>
+  </si>
+  <si>
+    <t>11,14th Naïve Bayes Algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensemble Learning Algo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start SQL book, 17th python sql integration </t>
+  </si>
+  <si>
+    <t>DIBETIC PREDICTION</t>
+  </si>
+  <si>
+    <t>HEATLTH and WEIGHT</t>
   </si>
 </sst>
 </file>
@@ -558,24 +588,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="30.88671875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="64" customWidth="1"/>
-    <col min="9" max="9" width="28.109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -592,7 +622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>45716</v>
       </c>
@@ -603,7 +633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>45716</v>
       </c>
@@ -614,7 +644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>45716</v>
       </c>
@@ -625,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>45716</v>
       </c>
@@ -639,7 +669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>45716</v>
       </c>
@@ -650,7 +680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>45716</v>
       </c>
@@ -664,7 +694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>45716</v>
       </c>
@@ -675,7 +705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>45716</v>
       </c>
@@ -686,7 +716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>45734</v>
       </c>
@@ -697,7 +727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>45734</v>
       </c>
@@ -708,7 +738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>45734</v>
       </c>
@@ -725,7 +755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>45734</v>
       </c>
@@ -736,7 +766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>45736</v>
       </c>
@@ -756,7 +786,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>45736</v>
       </c>
@@ -770,7 +800,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>45737</v>
       </c>
@@ -787,7 +817,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>45738</v>
       </c>
@@ -801,7 +831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>45740</v>
       </c>
@@ -812,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>45741</v>
       </c>
@@ -823,7 +853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>45740</v>
       </c>
@@ -834,7 +864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>45742</v>
       </c>
@@ -845,7 +875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>45743</v>
       </c>
@@ -859,7 +889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>45750</v>
       </c>
@@ -873,7 +903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>45756</v>
       </c>
@@ -884,7 +914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>45757</v>
       </c>
@@ -895,7 +925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>45757</v>
       </c>
@@ -906,7 +936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>45758</v>
       </c>
@@ -916,17 +946,103 @@
       <c r="C28" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>45761</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>45762</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>45768</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>45768</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>45768</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>45768</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>45768</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C3:C28">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="To be done">
+  <conditionalFormatting sqref="C3:C35">
+    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="To be done">
       <formula>NOT(ISERROR(SEARCH("To be done",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Completed">
+    <cfRule type="containsText" dxfId="0" priority="9" operator="containsText" text="Completed">
       <formula>NOT(ISERROR(SEARCH("Completed",C3)))</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -938,7 +1054,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C28" xr:uid="{5227195A-E2B1-46B7-86B4-E9F563518913}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C35" xr:uid="{5227195A-E2B1-46B7-86B4-E9F563518913}">
       <formula1>"To be done,Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>